<commit_message>
new temperature data and population data
</commit_message>
<xml_diff>
--- a/Available Data/Portland_Monthly_Avg_Precipitation.xlsx
+++ b/Available Data/Portland_Monthly_Avg_Precipitation.xlsx
@@ -8,19 +8,20 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\RDEL1VMM\Desktop\current projects\Maine_Blue_Economy\Available Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{FBAF970B-D2FC-4479-B64E-A5665B6C4152}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A263335E-660E-4136-8058-B4054B6861BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38510" yWindow="-15730" windowWidth="38620" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="17">
   <si>
     <t>Year</t>
   </si>
@@ -62,6 +63,15 @@
   </si>
   <si>
     <t>Annual</t>
+  </si>
+  <si>
+    <t>Monthly Total Precipitation for BELFAST, ME</t>
+  </si>
+  <si>
+    <t>Click column heading to sort ascending, click again to sort descending.</t>
+  </si>
+  <si>
+    <t>M</t>
   </si>
 </sst>
 </file>
@@ -449,7 +459,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D57BC25B-061C-4E92-9379-D5AE34D06A59}">
   <dimension ref="A1:N71"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="R17" sqref="R17"/>
     </sheetView>
   </sheetViews>
@@ -3583,4 +3593,3197 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6B3B5F34-2C19-47B0-8CDA-C607D12E6B0E}">
+  <dimension ref="A1:N74"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
+      <selection activeCell="G78" sqref="G78"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E3" t="s">
+        <v>4</v>
+      </c>
+      <c r="F3" t="s">
+        <v>5</v>
+      </c>
+      <c r="G3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H3" t="s">
+        <v>7</v>
+      </c>
+      <c r="I3" t="s">
+        <v>8</v>
+      </c>
+      <c r="J3" t="s">
+        <v>9</v>
+      </c>
+      <c r="K3" t="s">
+        <v>10</v>
+      </c>
+      <c r="L3" t="s">
+        <v>11</v>
+      </c>
+      <c r="M3" t="s">
+        <v>12</v>
+      </c>
+      <c r="N3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>1950</v>
+      </c>
+      <c r="B4">
+        <v>5.45</v>
+      </c>
+      <c r="C4">
+        <v>2.83</v>
+      </c>
+      <c r="D4">
+        <v>2.7</v>
+      </c>
+      <c r="E4">
+        <v>4.66</v>
+      </c>
+      <c r="F4">
+        <v>0.54</v>
+      </c>
+      <c r="G4">
+        <v>2.36</v>
+      </c>
+      <c r="H4">
+        <v>1.59</v>
+      </c>
+      <c r="I4">
+        <v>2.89</v>
+      </c>
+      <c r="J4">
+        <v>1.5</v>
+      </c>
+      <c r="K4">
+        <v>2.72</v>
+      </c>
+      <c r="L4">
+        <v>11.4</v>
+      </c>
+      <c r="M4">
+        <v>7.39</v>
+      </c>
+      <c r="N4">
+        <v>46.03</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>1951</v>
+      </c>
+      <c r="B5">
+        <v>4.24</v>
+      </c>
+      <c r="C5">
+        <v>5.48</v>
+      </c>
+      <c r="D5">
+        <v>5.4</v>
+      </c>
+      <c r="E5">
+        <v>5.72</v>
+      </c>
+      <c r="F5">
+        <v>3.45</v>
+      </c>
+      <c r="G5">
+        <v>1.85</v>
+      </c>
+      <c r="H5">
+        <v>8.0299999999999994</v>
+      </c>
+      <c r="I5">
+        <v>3.12</v>
+      </c>
+      <c r="J5">
+        <v>2.3199999999999998</v>
+      </c>
+      <c r="K5">
+        <v>5.3</v>
+      </c>
+      <c r="L5">
+        <v>10.44</v>
+      </c>
+      <c r="M5">
+        <v>6.4</v>
+      </c>
+      <c r="N5">
+        <v>61.75</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>1952</v>
+      </c>
+      <c r="B6">
+        <v>7.05</v>
+      </c>
+      <c r="C6">
+        <v>5.98</v>
+      </c>
+      <c r="D6">
+        <v>2.69</v>
+      </c>
+      <c r="E6">
+        <v>2.46</v>
+      </c>
+      <c r="F6">
+        <v>4.09</v>
+      </c>
+      <c r="G6">
+        <v>3.41</v>
+      </c>
+      <c r="H6">
+        <v>0.35</v>
+      </c>
+      <c r="I6">
+        <v>3.51</v>
+      </c>
+      <c r="J6">
+        <v>3.34</v>
+      </c>
+      <c r="K6">
+        <v>2.15</v>
+      </c>
+      <c r="L6">
+        <v>3.11</v>
+      </c>
+      <c r="M6">
+        <v>4.43</v>
+      </c>
+      <c r="N6">
+        <v>42.57</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>1953</v>
+      </c>
+      <c r="B7">
+        <v>6.57</v>
+      </c>
+      <c r="C7">
+        <v>4.76</v>
+      </c>
+      <c r="D7">
+        <v>10.59</v>
+      </c>
+      <c r="E7">
+        <v>5.8</v>
+      </c>
+      <c r="F7">
+        <v>3.09</v>
+      </c>
+      <c r="G7">
+        <v>3.04</v>
+      </c>
+      <c r="H7">
+        <v>4.91</v>
+      </c>
+      <c r="I7">
+        <v>2.44</v>
+      </c>
+      <c r="J7">
+        <v>3.98</v>
+      </c>
+      <c r="K7">
+        <v>6.23</v>
+      </c>
+      <c r="L7">
+        <v>5.22</v>
+      </c>
+      <c r="M7">
+        <v>6.12</v>
+      </c>
+      <c r="N7">
+        <v>62.75</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>1954</v>
+      </c>
+      <c r="B8">
+        <v>3.97</v>
+      </c>
+      <c r="C8">
+        <v>3.88</v>
+      </c>
+      <c r="D8">
+        <v>4.93</v>
+      </c>
+      <c r="E8">
+        <v>3.97</v>
+      </c>
+      <c r="F8">
+        <v>6.63</v>
+      </c>
+      <c r="G8">
+        <v>2.63</v>
+      </c>
+      <c r="H8">
+        <v>2.02</v>
+      </c>
+      <c r="I8">
+        <v>5.12</v>
+      </c>
+      <c r="J8">
+        <v>10.57</v>
+      </c>
+      <c r="K8">
+        <v>5.21</v>
+      </c>
+      <c r="L8">
+        <v>5.65</v>
+      </c>
+      <c r="M8">
+        <v>6.98</v>
+      </c>
+      <c r="N8">
+        <v>61.56</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>1955</v>
+      </c>
+      <c r="B9">
+        <v>1.52</v>
+      </c>
+      <c r="C9">
+        <v>7.86</v>
+      </c>
+      <c r="D9">
+        <v>5.63</v>
+      </c>
+      <c r="E9">
+        <v>2.46</v>
+      </c>
+      <c r="F9">
+        <v>2.04</v>
+      </c>
+      <c r="G9">
+        <v>3.34</v>
+      </c>
+      <c r="H9">
+        <v>1.1399999999999999</v>
+      </c>
+      <c r="I9">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="J9">
+        <v>2.34</v>
+      </c>
+      <c r="K9">
+        <v>3.16</v>
+      </c>
+      <c r="L9">
+        <v>6.73</v>
+      </c>
+      <c r="M9">
+        <v>1.18</v>
+      </c>
+      <c r="N9">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>1956</v>
+      </c>
+      <c r="B10">
+        <v>5.25</v>
+      </c>
+      <c r="C10">
+        <v>3.13</v>
+      </c>
+      <c r="D10">
+        <v>3.84</v>
+      </c>
+      <c r="E10">
+        <v>3.44</v>
+      </c>
+      <c r="F10">
+        <v>3.14</v>
+      </c>
+      <c r="G10">
+        <v>1.22</v>
+      </c>
+      <c r="H10">
+        <v>4.83</v>
+      </c>
+      <c r="I10">
+        <v>2.35</v>
+      </c>
+      <c r="J10">
+        <v>4.34</v>
+      </c>
+      <c r="K10">
+        <v>4.0199999999999996</v>
+      </c>
+      <c r="L10">
+        <v>4.17</v>
+      </c>
+      <c r="M10">
+        <v>5.0199999999999996</v>
+      </c>
+      <c r="N10">
+        <v>44.75</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>1957</v>
+      </c>
+      <c r="B11">
+        <v>2.65</v>
+      </c>
+      <c r="C11">
+        <v>1.45</v>
+      </c>
+      <c r="D11">
+        <v>3.21</v>
+      </c>
+      <c r="E11">
+        <v>2.93</v>
+      </c>
+      <c r="F11">
+        <v>2.39</v>
+      </c>
+      <c r="G11">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="H11">
+        <v>2.58</v>
+      </c>
+      <c r="I11">
+        <v>2.38</v>
+      </c>
+      <c r="J11">
+        <v>1.96</v>
+      </c>
+      <c r="K11">
+        <v>2.12</v>
+      </c>
+      <c r="L11">
+        <v>5.13</v>
+      </c>
+      <c r="M11">
+        <v>5.63</v>
+      </c>
+      <c r="N11">
+        <v>34.729999999999997</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>1958</v>
+      </c>
+      <c r="B12">
+        <v>8.9700000000000006</v>
+      </c>
+      <c r="C12">
+        <v>2.63</v>
+      </c>
+      <c r="D12">
+        <v>2.48</v>
+      </c>
+      <c r="E12">
+        <v>5.87</v>
+      </c>
+      <c r="F12">
+        <v>4.25</v>
+      </c>
+      <c r="G12">
+        <v>2.67</v>
+      </c>
+      <c r="H12">
+        <v>8.7100000000000009</v>
+      </c>
+      <c r="I12">
+        <v>4.59</v>
+      </c>
+      <c r="J12">
+        <v>3.55</v>
+      </c>
+      <c r="K12">
+        <v>6.63</v>
+      </c>
+      <c r="L12">
+        <v>6.48</v>
+      </c>
+      <c r="M12">
+        <v>2.04</v>
+      </c>
+      <c r="N12">
+        <v>58.87</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>1959</v>
+      </c>
+      <c r="B13">
+        <v>4.17</v>
+      </c>
+      <c r="C13">
+        <v>2.63</v>
+      </c>
+      <c r="D13">
+        <v>4.76</v>
+      </c>
+      <c r="E13">
+        <v>3.04</v>
+      </c>
+      <c r="F13">
+        <v>1.47</v>
+      </c>
+      <c r="G13">
+        <v>6.71</v>
+      </c>
+      <c r="H13">
+        <v>2.98</v>
+      </c>
+      <c r="I13">
+        <v>3.29</v>
+      </c>
+      <c r="J13">
+        <v>3.69</v>
+      </c>
+      <c r="K13">
+        <v>8.66</v>
+      </c>
+      <c r="L13">
+        <v>8.51</v>
+      </c>
+      <c r="M13">
+        <v>4.67</v>
+      </c>
+      <c r="N13">
+        <v>54.58</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>1960</v>
+      </c>
+      <c r="B14">
+        <v>4.03</v>
+      </c>
+      <c r="C14">
+        <v>7.42</v>
+      </c>
+      <c r="D14">
+        <v>2.5299999999999998</v>
+      </c>
+      <c r="E14">
+        <v>3.54</v>
+      </c>
+      <c r="F14">
+        <v>7.14</v>
+      </c>
+      <c r="G14">
+        <v>3.38</v>
+      </c>
+      <c r="H14">
+        <v>3.87</v>
+      </c>
+      <c r="I14">
+        <v>2.2400000000000002</v>
+      </c>
+      <c r="J14">
+        <v>4.04</v>
+      </c>
+      <c r="K14">
+        <v>3.46</v>
+      </c>
+      <c r="L14">
+        <v>4.07</v>
+      </c>
+      <c r="M14">
+        <v>7.05</v>
+      </c>
+      <c r="N14">
+        <v>52.77</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>1961</v>
+      </c>
+      <c r="B15">
+        <v>2.58</v>
+      </c>
+      <c r="C15">
+        <v>3.55</v>
+      </c>
+      <c r="D15">
+        <v>3.37</v>
+      </c>
+      <c r="E15">
+        <v>5.66</v>
+      </c>
+      <c r="F15">
+        <v>6.46</v>
+      </c>
+      <c r="G15">
+        <v>3.03</v>
+      </c>
+      <c r="H15">
+        <v>4.97</v>
+      </c>
+      <c r="I15">
+        <v>1.39</v>
+      </c>
+      <c r="J15">
+        <v>4.37</v>
+      </c>
+      <c r="K15">
+        <v>3.57</v>
+      </c>
+      <c r="L15">
+        <v>7.73</v>
+      </c>
+      <c r="M15">
+        <v>5.46</v>
+      </c>
+      <c r="N15">
+        <v>52.14</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>1962</v>
+      </c>
+      <c r="B16">
+        <v>3.69</v>
+      </c>
+      <c r="C16">
+        <v>1.98</v>
+      </c>
+      <c r="D16">
+        <v>1.5</v>
+      </c>
+      <c r="E16">
+        <v>5.57</v>
+      </c>
+      <c r="F16">
+        <v>1.58</v>
+      </c>
+      <c r="G16">
+        <v>2.5099999999999998</v>
+      </c>
+      <c r="H16">
+        <v>2.35</v>
+      </c>
+      <c r="I16">
+        <v>1.9</v>
+      </c>
+      <c r="J16">
+        <v>4.8499999999999996</v>
+      </c>
+      <c r="K16">
+        <v>6.99</v>
+      </c>
+      <c r="L16">
+        <v>7.45</v>
+      </c>
+      <c r="M16">
+        <v>6.69</v>
+      </c>
+      <c r="N16">
+        <v>47.06</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>1963</v>
+      </c>
+      <c r="B17">
+        <v>3.92</v>
+      </c>
+      <c r="C17">
+        <v>4.26</v>
+      </c>
+      <c r="D17">
+        <v>4.09</v>
+      </c>
+      <c r="E17">
+        <v>2.5299999999999998</v>
+      </c>
+      <c r="F17">
+        <v>5.97</v>
+      </c>
+      <c r="G17">
+        <v>1.08</v>
+      </c>
+      <c r="H17">
+        <v>1.98</v>
+      </c>
+      <c r="I17">
+        <v>3.74</v>
+      </c>
+      <c r="J17">
+        <v>2.64</v>
+      </c>
+      <c r="K17">
+        <v>3.98</v>
+      </c>
+      <c r="L17">
+        <v>10.06</v>
+      </c>
+      <c r="M17">
+        <v>2.38</v>
+      </c>
+      <c r="N17">
+        <v>46.63</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>1964</v>
+      </c>
+      <c r="B18">
+        <v>5.82</v>
+      </c>
+      <c r="C18">
+        <v>2.2400000000000002</v>
+      </c>
+      <c r="D18" t="s">
+        <v>16</v>
+      </c>
+      <c r="E18">
+        <v>3.54</v>
+      </c>
+      <c r="F18">
+        <v>1.38</v>
+      </c>
+      <c r="G18">
+        <v>2.54</v>
+      </c>
+      <c r="H18">
+        <v>2.41</v>
+      </c>
+      <c r="I18">
+        <v>3.94</v>
+      </c>
+      <c r="J18">
+        <v>1.62</v>
+      </c>
+      <c r="K18">
+        <v>3.38</v>
+      </c>
+      <c r="L18">
+        <v>3.43</v>
+      </c>
+      <c r="M18">
+        <v>4.49</v>
+      </c>
+      <c r="N18" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>1965</v>
+      </c>
+      <c r="B19">
+        <v>1.26</v>
+      </c>
+      <c r="C19" t="s">
+        <v>16</v>
+      </c>
+      <c r="D19">
+        <v>0.25</v>
+      </c>
+      <c r="E19">
+        <v>3.5</v>
+      </c>
+      <c r="F19">
+        <v>1.64</v>
+      </c>
+      <c r="G19">
+        <v>1.48</v>
+      </c>
+      <c r="H19">
+        <v>0.32</v>
+      </c>
+      <c r="I19">
+        <v>1.4</v>
+      </c>
+      <c r="J19">
+        <v>2.2400000000000002</v>
+      </c>
+      <c r="K19">
+        <v>6.13</v>
+      </c>
+      <c r="L19">
+        <v>4.76</v>
+      </c>
+      <c r="M19">
+        <v>3.05</v>
+      </c>
+      <c r="N19" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>1966</v>
+      </c>
+      <c r="B20">
+        <v>4.03</v>
+      </c>
+      <c r="C20">
+        <v>3.25</v>
+      </c>
+      <c r="D20">
+        <v>3.79</v>
+      </c>
+      <c r="E20">
+        <v>0.7</v>
+      </c>
+      <c r="F20">
+        <v>2.76</v>
+      </c>
+      <c r="G20">
+        <v>2.85</v>
+      </c>
+      <c r="H20">
+        <v>2.2400000000000002</v>
+      </c>
+      <c r="I20">
+        <v>3.1</v>
+      </c>
+      <c r="J20">
+        <v>3.21</v>
+      </c>
+      <c r="K20">
+        <v>4.01</v>
+      </c>
+      <c r="L20">
+        <v>8.06</v>
+      </c>
+      <c r="M20">
+        <v>3.45</v>
+      </c>
+      <c r="N20">
+        <v>41.45</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>1967</v>
+      </c>
+      <c r="B21">
+        <v>1.6</v>
+      </c>
+      <c r="C21">
+        <v>3.37</v>
+      </c>
+      <c r="D21">
+        <v>2.0099999999999998</v>
+      </c>
+      <c r="E21">
+        <v>2.9</v>
+      </c>
+      <c r="F21">
+        <v>4.5</v>
+      </c>
+      <c r="G21">
+        <v>4.9400000000000004</v>
+      </c>
+      <c r="H21">
+        <v>2.36</v>
+      </c>
+      <c r="I21">
+        <v>4.3099999999999996</v>
+      </c>
+      <c r="J21">
+        <v>2.79</v>
+      </c>
+      <c r="K21">
+        <v>2.59</v>
+      </c>
+      <c r="L21">
+        <v>2.92</v>
+      </c>
+      <c r="M21">
+        <v>6.77</v>
+      </c>
+      <c r="N21">
+        <v>41.06</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>1968</v>
+      </c>
+      <c r="B22">
+        <v>4.6900000000000004</v>
+      </c>
+      <c r="C22">
+        <v>1.85</v>
+      </c>
+      <c r="D22">
+        <v>4.24</v>
+      </c>
+      <c r="E22">
+        <v>2.66</v>
+      </c>
+      <c r="F22">
+        <v>4.9800000000000004</v>
+      </c>
+      <c r="G22">
+        <v>3.76</v>
+      </c>
+      <c r="H22">
+        <v>0.81</v>
+      </c>
+      <c r="I22">
+        <v>1.79</v>
+      </c>
+      <c r="J22">
+        <v>1.59</v>
+      </c>
+      <c r="K22">
+        <v>2.97</v>
+      </c>
+      <c r="L22">
+        <v>8.06</v>
+      </c>
+      <c r="M22">
+        <v>6.95</v>
+      </c>
+      <c r="N22">
+        <v>44.35</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>1969</v>
+      </c>
+      <c r="B23">
+        <v>2.89</v>
+      </c>
+      <c r="C23">
+        <v>6.16</v>
+      </c>
+      <c r="D23">
+        <v>2.5</v>
+      </c>
+      <c r="E23">
+        <v>3.38</v>
+      </c>
+      <c r="F23">
+        <v>1.81</v>
+      </c>
+      <c r="G23">
+        <v>2.0699999999999998</v>
+      </c>
+      <c r="H23">
+        <v>7.33</v>
+      </c>
+      <c r="I23">
+        <v>3.11</v>
+      </c>
+      <c r="J23">
+        <v>5.16</v>
+      </c>
+      <c r="K23">
+        <v>1.76</v>
+      </c>
+      <c r="L23">
+        <v>6.8</v>
+      </c>
+      <c r="M23">
+        <v>9.8000000000000007</v>
+      </c>
+      <c r="N23">
+        <v>52.77</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>1970</v>
+      </c>
+      <c r="B24">
+        <v>0.85</v>
+      </c>
+      <c r="C24">
+        <v>6.12</v>
+      </c>
+      <c r="D24">
+        <v>2.5099999999999998</v>
+      </c>
+      <c r="E24">
+        <v>3.96</v>
+      </c>
+      <c r="F24">
+        <v>3.19</v>
+      </c>
+      <c r="G24">
+        <v>3.06</v>
+      </c>
+      <c r="H24">
+        <v>0.78</v>
+      </c>
+      <c r="I24">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="J24">
+        <v>2.6</v>
+      </c>
+      <c r="K24">
+        <v>5.38</v>
+      </c>
+      <c r="L24">
+        <v>3.02</v>
+      </c>
+      <c r="M24">
+        <v>4.37</v>
+      </c>
+      <c r="N24">
+        <v>40.44</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>1971</v>
+      </c>
+      <c r="B25">
+        <v>2.4700000000000002</v>
+      </c>
+      <c r="C25">
+        <v>3.72</v>
+      </c>
+      <c r="D25">
+        <v>2.08</v>
+      </c>
+      <c r="E25">
+        <v>1.87</v>
+      </c>
+      <c r="F25">
+        <v>4.62</v>
+      </c>
+      <c r="G25">
+        <v>0.85</v>
+      </c>
+      <c r="H25">
+        <v>5.51</v>
+      </c>
+      <c r="I25">
+        <v>2.5099999999999998</v>
+      </c>
+      <c r="J25">
+        <v>3.19</v>
+      </c>
+      <c r="K25">
+        <v>3.79</v>
+      </c>
+      <c r="L25">
+        <v>3.42</v>
+      </c>
+      <c r="M25">
+        <v>3.09</v>
+      </c>
+      <c r="N25">
+        <v>37.119999999999997</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>1972</v>
+      </c>
+      <c r="B26">
+        <v>2.2799999999999998</v>
+      </c>
+      <c r="C26">
+        <v>5.33</v>
+      </c>
+      <c r="D26">
+        <v>9.9499999999999993</v>
+      </c>
+      <c r="E26">
+        <v>3.51</v>
+      </c>
+      <c r="F26">
+        <v>4.04</v>
+      </c>
+      <c r="G26">
+        <v>7.22</v>
+      </c>
+      <c r="H26">
+        <v>2.46</v>
+      </c>
+      <c r="I26">
+        <v>1.06</v>
+      </c>
+      <c r="J26">
+        <v>6.03</v>
+      </c>
+      <c r="K26">
+        <v>5.16</v>
+      </c>
+      <c r="L26">
+        <v>6.9</v>
+      </c>
+      <c r="M26">
+        <v>7.63</v>
+      </c>
+      <c r="N26">
+        <v>61.57</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>1973</v>
+      </c>
+      <c r="B27">
+        <v>2.2599999999999998</v>
+      </c>
+      <c r="C27">
+        <v>2.85</v>
+      </c>
+      <c r="D27">
+        <v>4.04</v>
+      </c>
+      <c r="E27">
+        <v>7.22</v>
+      </c>
+      <c r="F27">
+        <v>6.17</v>
+      </c>
+      <c r="G27">
+        <v>3.91</v>
+      </c>
+      <c r="H27">
+        <v>5.61</v>
+      </c>
+      <c r="I27">
+        <v>5.14</v>
+      </c>
+      <c r="J27">
+        <v>4.3600000000000003</v>
+      </c>
+      <c r="K27">
+        <v>4.1100000000000003</v>
+      </c>
+      <c r="L27">
+        <v>3.33</v>
+      </c>
+      <c r="M27">
+        <v>10.130000000000001</v>
+      </c>
+      <c r="N27">
+        <v>59.13</v>
+      </c>
+    </row>
+    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>1974</v>
+      </c>
+      <c r="B28">
+        <v>2.83</v>
+      </c>
+      <c r="C28">
+        <v>3.55</v>
+      </c>
+      <c r="D28">
+        <v>5.26</v>
+      </c>
+      <c r="E28">
+        <v>5.36</v>
+      </c>
+      <c r="F28">
+        <v>6.51</v>
+      </c>
+      <c r="G28">
+        <v>3.95</v>
+      </c>
+      <c r="H28">
+        <v>2.33</v>
+      </c>
+      <c r="I28">
+        <v>3</v>
+      </c>
+      <c r="J28">
+        <v>5.89</v>
+      </c>
+      <c r="K28">
+        <v>1.44</v>
+      </c>
+      <c r="L28">
+        <v>5.5</v>
+      </c>
+      <c r="M28">
+        <v>4.54</v>
+      </c>
+      <c r="N28">
+        <v>50.16</v>
+      </c>
+    </row>
+    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>1975</v>
+      </c>
+      <c r="B29">
+        <v>5.55</v>
+      </c>
+      <c r="C29">
+        <v>1.8</v>
+      </c>
+      <c r="D29">
+        <v>4.87</v>
+      </c>
+      <c r="E29">
+        <v>3.65</v>
+      </c>
+      <c r="F29">
+        <v>1.89</v>
+      </c>
+      <c r="G29">
+        <v>6.95</v>
+      </c>
+      <c r="H29">
+        <v>2.4300000000000002</v>
+      </c>
+      <c r="I29">
+        <v>2.38</v>
+      </c>
+      <c r="J29">
+        <v>5.2</v>
+      </c>
+      <c r="K29">
+        <v>5.18</v>
+      </c>
+      <c r="L29">
+        <v>7.16</v>
+      </c>
+      <c r="M29">
+        <v>7.96</v>
+      </c>
+      <c r="N29">
+        <v>55.02</v>
+      </c>
+    </row>
+    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>1976</v>
+      </c>
+      <c r="B30" t="s">
+        <v>16</v>
+      </c>
+      <c r="C30">
+        <v>3.99</v>
+      </c>
+      <c r="D30">
+        <v>3.01</v>
+      </c>
+      <c r="E30">
+        <v>4.7699999999999996</v>
+      </c>
+      <c r="F30">
+        <v>5.26</v>
+      </c>
+      <c r="G30">
+        <v>2.5299999999999998</v>
+      </c>
+      <c r="H30">
+        <v>5.12</v>
+      </c>
+      <c r="I30">
+        <v>2.85</v>
+      </c>
+      <c r="J30">
+        <v>1.05</v>
+      </c>
+      <c r="K30">
+        <v>6.95</v>
+      </c>
+      <c r="L30">
+        <v>1.97</v>
+      </c>
+      <c r="M30">
+        <v>4.67</v>
+      </c>
+      <c r="N30" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>1977</v>
+      </c>
+      <c r="B31">
+        <v>3.15</v>
+      </c>
+      <c r="C31">
+        <v>2.66</v>
+      </c>
+      <c r="D31">
+        <v>6.93</v>
+      </c>
+      <c r="E31">
+        <v>3.37</v>
+      </c>
+      <c r="F31">
+        <v>1.65</v>
+      </c>
+      <c r="G31">
+        <v>7.36</v>
+      </c>
+      <c r="H31">
+        <v>2.74</v>
+      </c>
+      <c r="I31">
+        <v>2.88</v>
+      </c>
+      <c r="J31">
+        <v>6.15</v>
+      </c>
+      <c r="K31">
+        <v>8.98</v>
+      </c>
+      <c r="L31">
+        <v>5.3</v>
+      </c>
+      <c r="M31">
+        <v>8.5</v>
+      </c>
+      <c r="N31">
+        <v>59.67</v>
+      </c>
+    </row>
+    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>1978</v>
+      </c>
+      <c r="B32">
+        <v>8.42</v>
+      </c>
+      <c r="C32">
+        <v>1.45</v>
+      </c>
+      <c r="D32">
+        <v>3.44</v>
+      </c>
+      <c r="E32">
+        <v>3.7</v>
+      </c>
+      <c r="F32">
+        <v>3.12</v>
+      </c>
+      <c r="G32">
+        <v>2.91</v>
+      </c>
+      <c r="H32">
+        <v>1.1599999999999999</v>
+      </c>
+      <c r="I32">
+        <v>1.38</v>
+      </c>
+      <c r="J32">
+        <v>0.94</v>
+      </c>
+      <c r="K32">
+        <v>5.57</v>
+      </c>
+      <c r="L32">
+        <v>2.0499999999999998</v>
+      </c>
+      <c r="M32">
+        <v>2.62</v>
+      </c>
+      <c r="N32">
+        <v>36.76</v>
+      </c>
+    </row>
+    <row r="33" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>1979</v>
+      </c>
+      <c r="B33">
+        <v>10.220000000000001</v>
+      </c>
+      <c r="C33">
+        <v>3.43</v>
+      </c>
+      <c r="D33">
+        <v>5.59</v>
+      </c>
+      <c r="E33">
+        <v>6.91</v>
+      </c>
+      <c r="F33">
+        <v>8.3699999999999992</v>
+      </c>
+      <c r="G33">
+        <v>1.2</v>
+      </c>
+      <c r="H33">
+        <v>1.65</v>
+      </c>
+      <c r="I33">
+        <v>4.2</v>
+      </c>
+      <c r="J33">
+        <v>4.09</v>
+      </c>
+      <c r="K33">
+        <v>6.97</v>
+      </c>
+      <c r="L33">
+        <v>5.17</v>
+      </c>
+      <c r="M33">
+        <v>2.93</v>
+      </c>
+      <c r="N33">
+        <v>60.73</v>
+      </c>
+    </row>
+    <row r="34" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>1980</v>
+      </c>
+      <c r="B34">
+        <v>1.82</v>
+      </c>
+      <c r="C34">
+        <v>1.29</v>
+      </c>
+      <c r="D34">
+        <v>5.66</v>
+      </c>
+      <c r="E34">
+        <v>6.75</v>
+      </c>
+      <c r="F34">
+        <v>1.95</v>
+      </c>
+      <c r="G34">
+        <v>2.97</v>
+      </c>
+      <c r="H34">
+        <v>5.82</v>
+      </c>
+      <c r="I34">
+        <v>1.24</v>
+      </c>
+      <c r="J34">
+        <v>4.78</v>
+      </c>
+      <c r="K34">
+        <v>4.33</v>
+      </c>
+      <c r="L34" t="s">
+        <v>16</v>
+      </c>
+      <c r="M34">
+        <v>2.36</v>
+      </c>
+      <c r="N34" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="35" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>1981</v>
+      </c>
+      <c r="B35">
+        <v>0.79</v>
+      </c>
+      <c r="C35">
+        <v>3.79</v>
+      </c>
+      <c r="D35">
+        <v>1.1399999999999999</v>
+      </c>
+      <c r="E35">
+        <v>4.2699999999999996</v>
+      </c>
+      <c r="F35">
+        <v>3.1</v>
+      </c>
+      <c r="G35">
+        <v>3.38</v>
+      </c>
+      <c r="H35">
+        <v>6.68</v>
+      </c>
+      <c r="I35">
+        <v>4.18</v>
+      </c>
+      <c r="J35">
+        <v>6.33</v>
+      </c>
+      <c r="K35">
+        <v>4.88</v>
+      </c>
+      <c r="L35">
+        <v>4.0199999999999996</v>
+      </c>
+      <c r="M35">
+        <v>6.05</v>
+      </c>
+      <c r="N35">
+        <v>48.61</v>
+      </c>
+    </row>
+    <row r="36" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <v>1982</v>
+      </c>
+      <c r="B36">
+        <v>4.91</v>
+      </c>
+      <c r="C36">
+        <v>3.09</v>
+      </c>
+      <c r="D36">
+        <v>2.12</v>
+      </c>
+      <c r="E36">
+        <v>5.28</v>
+      </c>
+      <c r="F36">
+        <v>1.65</v>
+      </c>
+      <c r="G36">
+        <v>4.82</v>
+      </c>
+      <c r="H36">
+        <v>2.68</v>
+      </c>
+      <c r="I36">
+        <v>2.93</v>
+      </c>
+      <c r="J36">
+        <v>1.59</v>
+      </c>
+      <c r="K36">
+        <v>1.69</v>
+      </c>
+      <c r="L36">
+        <v>5.59</v>
+      </c>
+      <c r="M36">
+        <v>1.58</v>
+      </c>
+      <c r="N36">
+        <v>37.93</v>
+      </c>
+    </row>
+    <row r="37" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <v>1983</v>
+      </c>
+      <c r="B37">
+        <v>3.86</v>
+      </c>
+      <c r="C37">
+        <v>3.24</v>
+      </c>
+      <c r="D37">
+        <v>8.33</v>
+      </c>
+      <c r="E37">
+        <v>13.67</v>
+      </c>
+      <c r="F37">
+        <v>6.26</v>
+      </c>
+      <c r="G37">
+        <v>0.92</v>
+      </c>
+      <c r="H37">
+        <v>3.84</v>
+      </c>
+      <c r="I37">
+        <v>3.65</v>
+      </c>
+      <c r="J37">
+        <v>1.48</v>
+      </c>
+      <c r="K37">
+        <v>3.94</v>
+      </c>
+      <c r="L37">
+        <v>12.88</v>
+      </c>
+      <c r="M37">
+        <v>9.2200000000000006</v>
+      </c>
+      <c r="N37">
+        <v>71.290000000000006</v>
+      </c>
+    </row>
+    <row r="38" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <v>1984</v>
+      </c>
+      <c r="B38">
+        <v>3.09</v>
+      </c>
+      <c r="C38">
+        <v>6.31</v>
+      </c>
+      <c r="D38">
+        <v>8.1999999999999993</v>
+      </c>
+      <c r="E38">
+        <v>4.1500000000000004</v>
+      </c>
+      <c r="F38">
+        <v>7.11</v>
+      </c>
+      <c r="G38">
+        <v>6.68</v>
+      </c>
+      <c r="H38">
+        <v>2.62</v>
+      </c>
+      <c r="I38">
+        <v>2.4</v>
+      </c>
+      <c r="J38">
+        <v>1.1599999999999999</v>
+      </c>
+      <c r="K38">
+        <v>3.02</v>
+      </c>
+      <c r="L38">
+        <v>2.04</v>
+      </c>
+      <c r="M38">
+        <v>3.88</v>
+      </c>
+      <c r="N38">
+        <v>50.66</v>
+      </c>
+    </row>
+    <row r="39" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A39">
+        <v>1985</v>
+      </c>
+      <c r="B39">
+        <v>1.1200000000000001</v>
+      </c>
+      <c r="C39">
+        <v>2.19</v>
+      </c>
+      <c r="D39">
+        <v>3.67</v>
+      </c>
+      <c r="E39">
+        <v>2.1800000000000002</v>
+      </c>
+      <c r="F39">
+        <v>3.99</v>
+      </c>
+      <c r="G39">
+        <v>3.2</v>
+      </c>
+      <c r="H39">
+        <v>1.76</v>
+      </c>
+      <c r="I39">
+        <v>6.82</v>
+      </c>
+      <c r="J39">
+        <v>3.07</v>
+      </c>
+      <c r="K39">
+        <v>3.4</v>
+      </c>
+      <c r="L39">
+        <v>6.29</v>
+      </c>
+      <c r="M39">
+        <v>2.0099999999999998</v>
+      </c>
+      <c r="N39" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="40" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A40">
+        <v>1986</v>
+      </c>
+      <c r="B40">
+        <v>4.82</v>
+      </c>
+      <c r="C40" t="s">
+        <v>16</v>
+      </c>
+      <c r="D40" t="s">
+        <v>16</v>
+      </c>
+      <c r="E40">
+        <v>3.98</v>
+      </c>
+      <c r="F40">
+        <v>3.86</v>
+      </c>
+      <c r="G40">
+        <v>2.54</v>
+      </c>
+      <c r="H40">
+        <v>4.37</v>
+      </c>
+      <c r="I40">
+        <v>6.25</v>
+      </c>
+      <c r="J40">
+        <v>3.11</v>
+      </c>
+      <c r="K40">
+        <v>1.64</v>
+      </c>
+      <c r="L40">
+        <v>4.03</v>
+      </c>
+      <c r="M40">
+        <v>4.4800000000000004</v>
+      </c>
+      <c r="N40" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="41" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A41">
+        <v>1987</v>
+      </c>
+      <c r="B41">
+        <v>3.61</v>
+      </c>
+      <c r="C41">
+        <v>0.92</v>
+      </c>
+      <c r="D41">
+        <v>3.84</v>
+      </c>
+      <c r="E41">
+        <v>6.24</v>
+      </c>
+      <c r="F41">
+        <v>3.37</v>
+      </c>
+      <c r="G41">
+        <v>3.58</v>
+      </c>
+      <c r="H41">
+        <v>1.51</v>
+      </c>
+      <c r="I41">
+        <v>2</v>
+      </c>
+      <c r="J41">
+        <v>8.02</v>
+      </c>
+      <c r="K41">
+        <v>3.09</v>
+      </c>
+      <c r="L41">
+        <v>3.43</v>
+      </c>
+      <c r="M41">
+        <v>3.13</v>
+      </c>
+      <c r="N41" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="42" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A42">
+        <v>1988</v>
+      </c>
+      <c r="B42" t="s">
+        <v>16</v>
+      </c>
+      <c r="C42">
+        <v>3.82</v>
+      </c>
+      <c r="D42">
+        <v>2.0299999999999998</v>
+      </c>
+      <c r="E42">
+        <v>3.18</v>
+      </c>
+      <c r="F42">
+        <v>3.22</v>
+      </c>
+      <c r="G42">
+        <v>2.09</v>
+      </c>
+      <c r="H42">
+        <v>4.47</v>
+      </c>
+      <c r="I42">
+        <v>5.17</v>
+      </c>
+      <c r="J42">
+        <v>1.62</v>
+      </c>
+      <c r="K42">
+        <v>4.12</v>
+      </c>
+      <c r="L42">
+        <v>7.75</v>
+      </c>
+      <c r="M42">
+        <v>1.1499999999999999</v>
+      </c>
+      <c r="N42" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="43" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A43">
+        <v>1989</v>
+      </c>
+      <c r="B43">
+        <v>1.29</v>
+      </c>
+      <c r="C43">
+        <v>2.88</v>
+      </c>
+      <c r="D43">
+        <v>2.75</v>
+      </c>
+      <c r="E43">
+        <v>3.76</v>
+      </c>
+      <c r="F43">
+        <v>9.84</v>
+      </c>
+      <c r="G43">
+        <v>5.75</v>
+      </c>
+      <c r="H43">
+        <v>1.45</v>
+      </c>
+      <c r="I43">
+        <v>2.94</v>
+      </c>
+      <c r="J43">
+        <v>4.9400000000000004</v>
+      </c>
+      <c r="K43">
+        <v>4.1399999999999997</v>
+      </c>
+      <c r="L43">
+        <v>6.63</v>
+      </c>
+      <c r="M43" t="s">
+        <v>16</v>
+      </c>
+      <c r="N43" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="44" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A44">
+        <v>1990</v>
+      </c>
+      <c r="B44">
+        <v>2.87</v>
+      </c>
+      <c r="C44">
+        <v>2.11</v>
+      </c>
+      <c r="D44">
+        <v>2.06</v>
+      </c>
+      <c r="E44">
+        <v>3.95</v>
+      </c>
+      <c r="F44">
+        <v>6.37</v>
+      </c>
+      <c r="G44">
+        <v>4.21</v>
+      </c>
+      <c r="H44">
+        <v>4.42</v>
+      </c>
+      <c r="I44">
+        <v>2.62</v>
+      </c>
+      <c r="J44">
+        <v>2.72</v>
+      </c>
+      <c r="K44">
+        <v>7.07</v>
+      </c>
+      <c r="L44">
+        <v>3.47</v>
+      </c>
+      <c r="M44">
+        <v>5.81</v>
+      </c>
+      <c r="N44">
+        <v>47.68</v>
+      </c>
+    </row>
+    <row r="45" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A45">
+        <v>1991</v>
+      </c>
+      <c r="B45">
+        <v>3.6</v>
+      </c>
+      <c r="C45">
+        <v>1.33</v>
+      </c>
+      <c r="D45">
+        <v>6.84</v>
+      </c>
+      <c r="E45">
+        <v>4.08</v>
+      </c>
+      <c r="F45" t="s">
+        <v>16</v>
+      </c>
+      <c r="G45">
+        <v>3.19</v>
+      </c>
+      <c r="H45">
+        <v>1.87</v>
+      </c>
+      <c r="I45">
+        <v>6.89</v>
+      </c>
+      <c r="J45">
+        <v>6.44</v>
+      </c>
+      <c r="K45">
+        <v>3.93</v>
+      </c>
+      <c r="L45">
+        <v>3.51</v>
+      </c>
+      <c r="M45" t="s">
+        <v>16</v>
+      </c>
+      <c r="N45" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="46" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A46">
+        <v>1992</v>
+      </c>
+      <c r="B46">
+        <v>7.31</v>
+      </c>
+      <c r="C46">
+        <v>4</v>
+      </c>
+      <c r="D46">
+        <v>3.89</v>
+      </c>
+      <c r="E46">
+        <v>2.77</v>
+      </c>
+      <c r="F46">
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="G46">
+        <v>3.15</v>
+      </c>
+      <c r="H46">
+        <v>2.82</v>
+      </c>
+      <c r="I46">
+        <v>2.8</v>
+      </c>
+      <c r="J46">
+        <v>2.38</v>
+      </c>
+      <c r="K46">
+        <v>3.62</v>
+      </c>
+      <c r="L46" t="s">
+        <v>16</v>
+      </c>
+      <c r="M46">
+        <v>2</v>
+      </c>
+      <c r="N46" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="47" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A47">
+        <v>1993</v>
+      </c>
+      <c r="B47" t="s">
+        <v>16</v>
+      </c>
+      <c r="C47">
+        <v>5.27</v>
+      </c>
+      <c r="D47" t="s">
+        <v>16</v>
+      </c>
+      <c r="E47">
+        <v>5.99</v>
+      </c>
+      <c r="F47" t="s">
+        <v>16</v>
+      </c>
+      <c r="G47">
+        <v>6.02</v>
+      </c>
+      <c r="H47">
+        <v>1.37</v>
+      </c>
+      <c r="I47">
+        <v>0.8</v>
+      </c>
+      <c r="J47">
+        <v>4.0599999999999996</v>
+      </c>
+      <c r="K47">
+        <v>3.82</v>
+      </c>
+      <c r="L47">
+        <v>6.41</v>
+      </c>
+      <c r="M47">
+        <v>6.29</v>
+      </c>
+      <c r="N47" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="48" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A48">
+        <v>1994</v>
+      </c>
+      <c r="B48">
+        <v>5.86</v>
+      </c>
+      <c r="C48" t="s">
+        <v>16</v>
+      </c>
+      <c r="D48">
+        <v>5.18</v>
+      </c>
+      <c r="E48">
+        <v>2.4500000000000002</v>
+      </c>
+      <c r="F48">
+        <v>4.45</v>
+      </c>
+      <c r="G48">
+        <v>3.74</v>
+      </c>
+      <c r="H48">
+        <v>2.71</v>
+      </c>
+      <c r="I48">
+        <v>3.34</v>
+      </c>
+      <c r="J48">
+        <v>9.16</v>
+      </c>
+      <c r="K48">
+        <v>3.88</v>
+      </c>
+      <c r="L48">
+        <v>4.59</v>
+      </c>
+      <c r="M48">
+        <v>4</v>
+      </c>
+      <c r="N48" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="49" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A49">
+        <v>1995</v>
+      </c>
+      <c r="B49">
+        <v>4.57</v>
+      </c>
+      <c r="C49">
+        <v>2.96</v>
+      </c>
+      <c r="D49">
+        <v>2.0299999999999998</v>
+      </c>
+      <c r="E49" t="s">
+        <v>16</v>
+      </c>
+      <c r="F49">
+        <v>4.66</v>
+      </c>
+      <c r="G49">
+        <v>6.55</v>
+      </c>
+      <c r="H49">
+        <v>3.12</v>
+      </c>
+      <c r="I49" t="s">
+        <v>16</v>
+      </c>
+      <c r="J49">
+        <v>2.91</v>
+      </c>
+      <c r="K49">
+        <v>5.32</v>
+      </c>
+      <c r="L49">
+        <v>7.03</v>
+      </c>
+      <c r="M49" t="s">
+        <v>16</v>
+      </c>
+      <c r="N49" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="50" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A50">
+        <v>1996</v>
+      </c>
+      <c r="B50">
+        <v>4.97</v>
+      </c>
+      <c r="C50">
+        <v>3.52</v>
+      </c>
+      <c r="D50">
+        <v>2.59</v>
+      </c>
+      <c r="E50" t="s">
+        <v>16</v>
+      </c>
+      <c r="F50" t="s">
+        <v>16</v>
+      </c>
+      <c r="G50" t="s">
+        <v>16</v>
+      </c>
+      <c r="H50">
+        <v>6.79</v>
+      </c>
+      <c r="I50">
+        <v>1.19</v>
+      </c>
+      <c r="J50">
+        <v>7.44</v>
+      </c>
+      <c r="K50">
+        <v>2.5299999999999998</v>
+      </c>
+      <c r="L50">
+        <v>2.5</v>
+      </c>
+      <c r="M50">
+        <v>6.5</v>
+      </c>
+      <c r="N50" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="51" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A51">
+        <v>1997</v>
+      </c>
+      <c r="B51">
+        <v>5.0599999999999996</v>
+      </c>
+      <c r="C51">
+        <v>1.78</v>
+      </c>
+      <c r="D51">
+        <v>3.9</v>
+      </c>
+      <c r="E51">
+        <v>3.66</v>
+      </c>
+      <c r="F51">
+        <v>3.02</v>
+      </c>
+      <c r="G51">
+        <v>3.4</v>
+      </c>
+      <c r="H51">
+        <v>3.03</v>
+      </c>
+      <c r="I51">
+        <v>2.46</v>
+      </c>
+      <c r="J51">
+        <v>2.39</v>
+      </c>
+      <c r="K51">
+        <v>1.21</v>
+      </c>
+      <c r="L51">
+        <v>3.81</v>
+      </c>
+      <c r="M51">
+        <v>2.6</v>
+      </c>
+      <c r="N51" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="52" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A52">
+        <v>1998</v>
+      </c>
+      <c r="B52" t="s">
+        <v>16</v>
+      </c>
+      <c r="C52">
+        <v>3.43</v>
+      </c>
+      <c r="D52">
+        <v>3.04</v>
+      </c>
+      <c r="E52">
+        <v>3.64</v>
+      </c>
+      <c r="F52">
+        <v>4.87</v>
+      </c>
+      <c r="G52">
+        <v>6.57</v>
+      </c>
+      <c r="H52">
+        <v>1.97</v>
+      </c>
+      <c r="I52">
+        <v>1.9</v>
+      </c>
+      <c r="J52">
+        <v>1.5</v>
+      </c>
+      <c r="K52">
+        <v>6.68</v>
+      </c>
+      <c r="L52">
+        <v>3.06</v>
+      </c>
+      <c r="M52">
+        <v>1.93</v>
+      </c>
+      <c r="N52" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="53" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A53">
+        <v>1999</v>
+      </c>
+      <c r="B53">
+        <v>6.69</v>
+      </c>
+      <c r="C53">
+        <v>3.85</v>
+      </c>
+      <c r="D53">
+        <v>6.68</v>
+      </c>
+      <c r="E53">
+        <v>0.37</v>
+      </c>
+      <c r="F53">
+        <v>3.38</v>
+      </c>
+      <c r="G53">
+        <v>1.66</v>
+      </c>
+      <c r="H53">
+        <v>0.71</v>
+      </c>
+      <c r="I53">
+        <v>1.74</v>
+      </c>
+      <c r="J53">
+        <v>9.76</v>
+      </c>
+      <c r="K53">
+        <v>5.15</v>
+      </c>
+      <c r="L53">
+        <v>3.56</v>
+      </c>
+      <c r="M53">
+        <v>3.09</v>
+      </c>
+      <c r="N53">
+        <v>46.64</v>
+      </c>
+    </row>
+    <row r="54" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A54">
+        <v>2000</v>
+      </c>
+      <c r="B54">
+        <v>3.58</v>
+      </c>
+      <c r="C54">
+        <v>2.31</v>
+      </c>
+      <c r="D54">
+        <v>3.47</v>
+      </c>
+      <c r="E54">
+        <v>5.87</v>
+      </c>
+      <c r="F54">
+        <v>5.5</v>
+      </c>
+      <c r="G54">
+        <v>4.0599999999999996</v>
+      </c>
+      <c r="H54">
+        <v>2.86</v>
+      </c>
+      <c r="I54">
+        <v>1.48</v>
+      </c>
+      <c r="J54">
+        <v>1.29</v>
+      </c>
+      <c r="K54">
+        <v>4.38</v>
+      </c>
+      <c r="L54">
+        <v>3.21</v>
+      </c>
+      <c r="M54">
+        <v>3.54</v>
+      </c>
+      <c r="N54">
+        <v>41.55</v>
+      </c>
+    </row>
+    <row r="55" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A55">
+        <v>2001</v>
+      </c>
+      <c r="B55">
+        <v>1.23</v>
+      </c>
+      <c r="C55">
+        <v>1.64</v>
+      </c>
+      <c r="D55">
+        <v>3.72</v>
+      </c>
+      <c r="E55">
+        <v>0.91</v>
+      </c>
+      <c r="F55">
+        <v>1.44</v>
+      </c>
+      <c r="G55" t="s">
+        <v>16</v>
+      </c>
+      <c r="H55">
+        <v>1.51</v>
+      </c>
+      <c r="I55">
+        <v>1.1599999999999999</v>
+      </c>
+      <c r="J55" t="s">
+        <v>16</v>
+      </c>
+      <c r="K55">
+        <v>1.41</v>
+      </c>
+      <c r="L55">
+        <v>2.4700000000000002</v>
+      </c>
+      <c r="M55">
+        <v>3.86</v>
+      </c>
+      <c r="N55" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="56" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A56">
+        <v>2002</v>
+      </c>
+      <c r="B56">
+        <v>2.86</v>
+      </c>
+      <c r="C56">
+        <v>3.41</v>
+      </c>
+      <c r="D56">
+        <v>4.05</v>
+      </c>
+      <c r="E56">
+        <v>6.42</v>
+      </c>
+      <c r="F56">
+        <v>3.51</v>
+      </c>
+      <c r="G56">
+        <v>3.32</v>
+      </c>
+      <c r="H56">
+        <v>2.33</v>
+      </c>
+      <c r="I56">
+        <v>1.04</v>
+      </c>
+      <c r="J56">
+        <v>5.43</v>
+      </c>
+      <c r="K56">
+        <v>2.57</v>
+      </c>
+      <c r="L56">
+        <v>6.02</v>
+      </c>
+      <c r="M56">
+        <v>4.88</v>
+      </c>
+      <c r="N56">
+        <v>45.84</v>
+      </c>
+    </row>
+    <row r="57" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A57">
+        <v>2003</v>
+      </c>
+      <c r="B57">
+        <v>1.2</v>
+      </c>
+      <c r="C57">
+        <v>2.78</v>
+      </c>
+      <c r="D57">
+        <v>4.2</v>
+      </c>
+      <c r="E57">
+        <v>1.94</v>
+      </c>
+      <c r="F57">
+        <v>3.18</v>
+      </c>
+      <c r="G57">
+        <v>2.4500000000000002</v>
+      </c>
+      <c r="H57">
+        <v>1.37</v>
+      </c>
+      <c r="I57">
+        <v>2.34</v>
+      </c>
+      <c r="J57">
+        <v>6.07</v>
+      </c>
+      <c r="K57">
+        <v>6.87</v>
+      </c>
+      <c r="L57">
+        <v>5</v>
+      </c>
+      <c r="M57">
+        <v>4.54</v>
+      </c>
+      <c r="N57">
+        <v>41.94</v>
+      </c>
+    </row>
+    <row r="58" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A58">
+        <v>2004</v>
+      </c>
+      <c r="B58">
+        <v>0.91</v>
+      </c>
+      <c r="C58">
+        <v>1.59</v>
+      </c>
+      <c r="D58">
+        <v>1.53</v>
+      </c>
+      <c r="E58">
+        <v>4.03</v>
+      </c>
+      <c r="F58">
+        <v>5.55</v>
+      </c>
+      <c r="G58">
+        <v>2.06</v>
+      </c>
+      <c r="H58">
+        <v>5.46</v>
+      </c>
+      <c r="I58">
+        <v>6.05</v>
+      </c>
+      <c r="J58">
+        <v>2.35</v>
+      </c>
+      <c r="K58">
+        <v>1.94</v>
+      </c>
+      <c r="L58">
+        <v>5.26</v>
+      </c>
+      <c r="M58">
+        <v>4.3600000000000003</v>
+      </c>
+      <c r="N58">
+        <v>41.09</v>
+      </c>
+    </row>
+    <row r="59" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A59">
+        <v>2005</v>
+      </c>
+      <c r="B59">
+        <v>2.86</v>
+      </c>
+      <c r="C59">
+        <v>3.21</v>
+      </c>
+      <c r="D59">
+        <v>4.8099999999999996</v>
+      </c>
+      <c r="E59">
+        <v>10.16</v>
+      </c>
+      <c r="F59">
+        <v>8.4600000000000009</v>
+      </c>
+      <c r="G59">
+        <v>2.97</v>
+      </c>
+      <c r="H59">
+        <v>3.15</v>
+      </c>
+      <c r="I59">
+        <v>3.42</v>
+      </c>
+      <c r="J59">
+        <v>2.99</v>
+      </c>
+      <c r="K59">
+        <v>16.190000000000001</v>
+      </c>
+      <c r="L59">
+        <v>7.49</v>
+      </c>
+      <c r="M59">
+        <v>5.44</v>
+      </c>
+      <c r="N59" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="60" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A60">
+        <v>2006</v>
+      </c>
+      <c r="B60">
+        <v>4.29</v>
+      </c>
+      <c r="C60">
+        <v>4.91</v>
+      </c>
+      <c r="D60">
+        <v>1.22</v>
+      </c>
+      <c r="E60">
+        <v>1.97</v>
+      </c>
+      <c r="F60">
+        <v>6.22</v>
+      </c>
+      <c r="G60">
+        <v>8.98</v>
+      </c>
+      <c r="H60">
+        <v>6.36</v>
+      </c>
+      <c r="I60">
+        <v>2.36</v>
+      </c>
+      <c r="J60">
+        <v>3.05</v>
+      </c>
+      <c r="K60">
+        <v>8</v>
+      </c>
+      <c r="L60">
+        <v>5.8</v>
+      </c>
+      <c r="M60">
+        <v>3.17</v>
+      </c>
+      <c r="N60">
+        <v>56.33</v>
+      </c>
+    </row>
+    <row r="61" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A61">
+        <v>2007</v>
+      </c>
+      <c r="B61">
+        <v>3.1</v>
+      </c>
+      <c r="C61">
+        <v>2.17</v>
+      </c>
+      <c r="D61">
+        <v>6.19</v>
+      </c>
+      <c r="E61">
+        <v>7.16</v>
+      </c>
+      <c r="F61">
+        <v>3.75</v>
+      </c>
+      <c r="G61">
+        <v>2.5</v>
+      </c>
+      <c r="H61">
+        <v>3.39</v>
+      </c>
+      <c r="I61">
+        <v>4.37</v>
+      </c>
+      <c r="J61">
+        <v>4.0199999999999996</v>
+      </c>
+      <c r="K61">
+        <v>6.43</v>
+      </c>
+      <c r="L61">
+        <v>6.47</v>
+      </c>
+      <c r="M61">
+        <v>4.66</v>
+      </c>
+      <c r="N61">
+        <v>54.21</v>
+      </c>
+    </row>
+    <row r="62" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A62">
+        <v>2008</v>
+      </c>
+      <c r="B62">
+        <v>3.02</v>
+      </c>
+      <c r="C62">
+        <v>7.42</v>
+      </c>
+      <c r="D62">
+        <v>5.2</v>
+      </c>
+      <c r="E62">
+        <v>5.15</v>
+      </c>
+      <c r="F62">
+        <v>2.34</v>
+      </c>
+      <c r="G62">
+        <v>3.26</v>
+      </c>
+      <c r="H62">
+        <v>3.97</v>
+      </c>
+      <c r="I62">
+        <v>4.9800000000000004</v>
+      </c>
+      <c r="J62">
+        <v>9.61</v>
+      </c>
+      <c r="K62">
+        <v>2.54</v>
+      </c>
+      <c r="L62">
+        <v>3.98</v>
+      </c>
+      <c r="M62">
+        <v>5.4</v>
+      </c>
+      <c r="N62" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="63" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A63">
+        <v>2009</v>
+      </c>
+      <c r="B63">
+        <v>3.2</v>
+      </c>
+      <c r="C63">
+        <v>2.65</v>
+      </c>
+      <c r="D63">
+        <v>3.01</v>
+      </c>
+      <c r="E63">
+        <v>7.54</v>
+      </c>
+      <c r="F63">
+        <v>5.08</v>
+      </c>
+      <c r="G63">
+        <v>7.9</v>
+      </c>
+      <c r="H63">
+        <v>8.0399999999999991</v>
+      </c>
+      <c r="I63">
+        <v>4.99</v>
+      </c>
+      <c r="J63">
+        <v>1.94</v>
+      </c>
+      <c r="K63">
+        <v>5.95</v>
+      </c>
+      <c r="L63">
+        <v>5.92</v>
+      </c>
+      <c r="M63">
+        <v>4.68</v>
+      </c>
+      <c r="N63" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="64" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A64">
+        <v>2010</v>
+      </c>
+      <c r="B64">
+        <v>5.72</v>
+      </c>
+      <c r="C64">
+        <v>2.78</v>
+      </c>
+      <c r="D64">
+        <v>8.1199999999999992</v>
+      </c>
+      <c r="E64">
+        <v>3.4</v>
+      </c>
+      <c r="F64">
+        <v>1.89</v>
+      </c>
+      <c r="G64">
+        <v>5.08</v>
+      </c>
+      <c r="H64">
+        <v>3.47</v>
+      </c>
+      <c r="I64">
+        <v>3.59</v>
+      </c>
+      <c r="J64">
+        <v>6.47</v>
+      </c>
+      <c r="K64">
+        <v>7.2</v>
+      </c>
+      <c r="L64">
+        <v>6.16</v>
+      </c>
+      <c r="M64">
+        <v>5.82</v>
+      </c>
+      <c r="N64">
+        <v>59.7</v>
+      </c>
+    </row>
+    <row r="65" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A65">
+        <v>2011</v>
+      </c>
+      <c r="B65">
+        <v>3.44</v>
+      </c>
+      <c r="C65">
+        <v>3.06</v>
+      </c>
+      <c r="D65">
+        <v>5.93</v>
+      </c>
+      <c r="E65">
+        <v>5.51</v>
+      </c>
+      <c r="F65">
+        <v>3.7</v>
+      </c>
+      <c r="G65">
+        <v>4.01</v>
+      </c>
+      <c r="H65">
+        <v>2.2599999999999998</v>
+      </c>
+      <c r="I65">
+        <v>6.79</v>
+      </c>
+      <c r="J65">
+        <v>2.64</v>
+      </c>
+      <c r="K65">
+        <v>6.84</v>
+      </c>
+      <c r="L65">
+        <v>3.06</v>
+      </c>
+      <c r="M65">
+        <v>4.25</v>
+      </c>
+      <c r="N65">
+        <v>51.49</v>
+      </c>
+    </row>
+    <row r="66" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A66">
+        <v>2012</v>
+      </c>
+      <c r="B66">
+        <v>2.9</v>
+      </c>
+      <c r="C66">
+        <v>1.27</v>
+      </c>
+      <c r="D66">
+        <v>2.31</v>
+      </c>
+      <c r="E66">
+        <v>4.8600000000000003</v>
+      </c>
+      <c r="F66">
+        <v>5.95</v>
+      </c>
+      <c r="G66">
+        <v>8.76</v>
+      </c>
+      <c r="H66">
+        <v>1.55</v>
+      </c>
+      <c r="I66">
+        <v>3.24</v>
+      </c>
+      <c r="J66">
+        <v>3.52</v>
+      </c>
+      <c r="K66">
+        <v>6.35</v>
+      </c>
+      <c r="L66">
+        <v>1.47</v>
+      </c>
+      <c r="M66">
+        <v>6.25</v>
+      </c>
+      <c r="N66">
+        <v>48.43</v>
+      </c>
+    </row>
+    <row r="67" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A67">
+        <v>2013</v>
+      </c>
+      <c r="B67">
+        <v>0.99</v>
+      </c>
+      <c r="C67">
+        <v>4.08</v>
+      </c>
+      <c r="D67">
+        <v>2.37</v>
+      </c>
+      <c r="E67">
+        <v>1.93</v>
+      </c>
+      <c r="F67">
+        <v>5.08</v>
+      </c>
+      <c r="G67">
+        <v>6.33</v>
+      </c>
+      <c r="H67">
+        <v>2.81</v>
+      </c>
+      <c r="I67">
+        <v>3.56</v>
+      </c>
+      <c r="J67">
+        <v>5.32</v>
+      </c>
+      <c r="K67">
+        <v>1.24</v>
+      </c>
+      <c r="L67">
+        <v>5.76</v>
+      </c>
+      <c r="M67">
+        <v>5.76</v>
+      </c>
+      <c r="N67">
+        <v>45.23</v>
+      </c>
+    </row>
+    <row r="68" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A68">
+        <v>2014</v>
+      </c>
+      <c r="B68">
+        <v>5.85</v>
+      </c>
+      <c r="C68">
+        <v>3.28</v>
+      </c>
+      <c r="D68">
+        <v>4.68</v>
+      </c>
+      <c r="E68">
+        <v>3.7</v>
+      </c>
+      <c r="F68">
+        <v>3.46</v>
+      </c>
+      <c r="G68">
+        <v>4.8899999999999997</v>
+      </c>
+      <c r="H68">
+        <v>8.07</v>
+      </c>
+      <c r="I68">
+        <v>3.37</v>
+      </c>
+      <c r="J68">
+        <v>1.47</v>
+      </c>
+      <c r="K68">
+        <v>7.43</v>
+      </c>
+      <c r="L68">
+        <v>5.67</v>
+      </c>
+      <c r="M68">
+        <v>6.72</v>
+      </c>
+      <c r="N68">
+        <v>58.59</v>
+      </c>
+    </row>
+    <row r="69" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A69">
+        <v>2015</v>
+      </c>
+      <c r="B69">
+        <v>4.1900000000000004</v>
+      </c>
+      <c r="C69">
+        <v>2.7</v>
+      </c>
+      <c r="D69">
+        <v>1.79</v>
+      </c>
+      <c r="E69">
+        <v>3.36</v>
+      </c>
+      <c r="F69">
+        <v>1.88</v>
+      </c>
+      <c r="G69">
+        <v>5.34</v>
+      </c>
+      <c r="H69">
+        <v>1.9</v>
+      </c>
+      <c r="I69">
+        <v>2.33</v>
+      </c>
+      <c r="J69">
+        <v>3.18</v>
+      </c>
+      <c r="K69">
+        <v>13.02</v>
+      </c>
+      <c r="L69">
+        <v>3.67</v>
+      </c>
+      <c r="M69">
+        <v>5.53</v>
+      </c>
+      <c r="N69">
+        <v>48.89</v>
+      </c>
+    </row>
+    <row r="70" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A70">
+        <v>2016</v>
+      </c>
+      <c r="B70">
+        <v>2.76</v>
+      </c>
+      <c r="C70">
+        <v>5.38</v>
+      </c>
+      <c r="D70">
+        <v>4.04</v>
+      </c>
+      <c r="E70">
+        <v>2.85</v>
+      </c>
+      <c r="F70">
+        <v>2.2400000000000002</v>
+      </c>
+      <c r="G70">
+        <v>3.28</v>
+      </c>
+      <c r="H70">
+        <v>3.62</v>
+      </c>
+      <c r="I70">
+        <v>1.59</v>
+      </c>
+      <c r="J70">
+        <v>2.38</v>
+      </c>
+      <c r="K70">
+        <v>4.6100000000000003</v>
+      </c>
+      <c r="L70">
+        <v>6.12</v>
+      </c>
+      <c r="M70">
+        <v>5.43</v>
+      </c>
+      <c r="N70">
+        <v>44.3</v>
+      </c>
+    </row>
+    <row r="71" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A71">
+        <v>2017</v>
+      </c>
+      <c r="B71">
+        <v>5.4</v>
+      </c>
+      <c r="C71">
+        <v>3.17</v>
+      </c>
+      <c r="D71">
+        <v>2.48</v>
+      </c>
+      <c r="E71">
+        <v>4.25</v>
+      </c>
+      <c r="F71">
+        <v>7.36</v>
+      </c>
+      <c r="G71">
+        <v>2.73</v>
+      </c>
+      <c r="H71">
+        <v>1.26</v>
+      </c>
+      <c r="I71">
+        <v>1.95</v>
+      </c>
+      <c r="J71">
+        <v>2.46</v>
+      </c>
+      <c r="K71">
+        <v>5.22</v>
+      </c>
+      <c r="L71">
+        <v>2.61</v>
+      </c>
+      <c r="M71">
+        <v>5.0199999999999996</v>
+      </c>
+      <c r="N71">
+        <v>43.91</v>
+      </c>
+    </row>
+    <row r="72" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A72">
+        <v>2018</v>
+      </c>
+      <c r="B72">
+        <v>5.78</v>
+      </c>
+      <c r="C72">
+        <v>4.3600000000000003</v>
+      </c>
+      <c r="D72">
+        <v>2.81</v>
+      </c>
+      <c r="E72">
+        <v>6.45</v>
+      </c>
+      <c r="F72">
+        <v>0.95</v>
+      </c>
+      <c r="G72">
+        <v>3.91</v>
+      </c>
+      <c r="H72">
+        <v>1.39</v>
+      </c>
+      <c r="I72">
+        <v>4.04</v>
+      </c>
+      <c r="J72">
+        <v>5.44</v>
+      </c>
+      <c r="K72">
+        <v>4.92</v>
+      </c>
+      <c r="L72">
+        <v>7.51</v>
+      </c>
+      <c r="M72">
+        <v>3.81</v>
+      </c>
+      <c r="N72">
+        <v>51.37</v>
+      </c>
+    </row>
+    <row r="73" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A73">
+        <v>2019</v>
+      </c>
+      <c r="B73">
+        <v>6.34</v>
+      </c>
+      <c r="C73">
+        <v>3.07</v>
+      </c>
+      <c r="D73">
+        <v>2.54</v>
+      </c>
+      <c r="E73">
+        <v>5.68</v>
+      </c>
+      <c r="F73">
+        <v>3.32</v>
+      </c>
+      <c r="G73">
+        <v>5.51</v>
+      </c>
+      <c r="H73">
+        <v>2.33</v>
+      </c>
+      <c r="I73">
+        <v>5.47</v>
+      </c>
+      <c r="J73">
+        <v>2.48</v>
+      </c>
+      <c r="K73">
+        <v>6.72</v>
+      </c>
+      <c r="L73">
+        <v>4.4800000000000004</v>
+      </c>
+      <c r="M73">
+        <v>5.59</v>
+      </c>
+      <c r="N73">
+        <v>53.53</v>
+      </c>
+    </row>
+    <row r="74" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A74">
+        <v>2020</v>
+      </c>
+      <c r="B74">
+        <v>3.41</v>
+      </c>
+      <c r="C74">
+        <v>2.91</v>
+      </c>
+      <c r="D74">
+        <v>2.81</v>
+      </c>
+      <c r="E74">
+        <v>5.51</v>
+      </c>
+      <c r="F74">
+        <v>3.7</v>
+      </c>
+      <c r="G74">
+        <v>2.86</v>
+      </c>
+      <c r="H74">
+        <v>2.31</v>
+      </c>
+      <c r="I74">
+        <v>2.41</v>
+      </c>
+      <c r="J74">
+        <v>0.89</v>
+      </c>
+      <c r="K74">
+        <v>5.31</v>
+      </c>
+      <c r="L74">
+        <v>4.25</v>
+      </c>
+      <c r="M74">
+        <v>6.52</v>
+      </c>
+      <c r="N74">
+        <v>42.89</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>